<commit_message>
refactor: simplify page object structure and implementation
- Remove method chaining from page objects (no longer return page instances)
- Make page object structure consistent across all classes
- Remove logging from page objects
- Clean up overall code organization in page classes

Next step: Review test classes and improve logging implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/signup_data.xlsx
+++ b/src/test/resources/testData/signup_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEPI\Project\Automation_Exercise\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95130604-776C-4346-AE3C-BC5A71E9EB5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D5D8E7-2360-4CD7-B816-A6BD91551568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{985B74B3-7B1C-4AC1-85EF-FEA90879A07F}"/>
   </bookViews>
@@ -503,7 +503,7 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="A1:XFD1048576"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>